<commit_message>
Fix on SHACL and little fixes on XSLT
</commit_message>
<xml_diff>
--- a/Subtask5/03-eli-dl-ap-ep-activities/04-SHACL/Activities-Shapes-Generic.xlsx
+++ b/Subtask5/03-eli-dl-ap-ep-activities/04-SHACL/Activities-Shapes-Generic.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="209">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -302,23 +302,7 @@
     <t xml:space="preserve">eli:Language</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/language/[A-Z]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[A-Z][A-Z]$"</t>
-    </r>
+    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/language/[A-Z][A-Z][A-Z]$"</t>
   </si>
   <si>
     <t xml:space="preserve">elidl-ep:Agent</t>
@@ -342,6 +326,12 @@
     <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/vote-mode/.*$"</t>
   </si>
   <si>
+    <t xml:space="preserve">elidl-ep:InvolvedWorkRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/involved-work-role/.*$"</t>
+  </si>
+  <si>
     <t xml:space="preserve">This sheet specifies constraints that are attached to the NodeShapes specified in the first sheet</t>
   </si>
   <si>
@@ -649,6 +639,15 @@
   </si>
   <si>
     <t xml:space="preserve">elidl-ep:voteAgainst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on InvolvedWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:involvedWorkRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elidl-ep:hasWorkInvolved</t>
   </si>
 </sst>
 </file>
@@ -718,11 +717,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -736,6 +730,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -880,15 +879,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -908,7 +907,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -990,22 +989,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K42" activeCellId="0" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.55"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="1" width="35.27"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="1" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="67.48"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="1" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="7" style="1" width="23.68"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="42.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="67.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="23.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="42.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="106.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.68"/>
@@ -1674,6 +1673,9 @@
       <c r="A34" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J34" s="1" t="s">
         <v>47</v>
       </c>
@@ -1688,6 +1690,9 @@
       <c r="A35" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1705,6 +1710,9 @@
       <c r="A36" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J36" s="1" t="s">
         <v>47</v>
       </c>
@@ -1719,6 +1727,9 @@
       <c r="A37" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1736,6 +1747,9 @@
       <c r="A38" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J38" s="1" t="s">
         <v>47</v>
       </c>
@@ -1750,6 +1764,9 @@
       <c r="A39" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>47</v>
       </c>
@@ -1767,6 +1784,9 @@
       <c r="A40" s="5" t="s">
         <v>99</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="J40" s="1" t="s">
         <v>47</v>
       </c>
@@ -1777,6 +1797,26 @@
         <v>49</v>
       </c>
       <c r="M40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1806,15 +1846,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="M77" activeCellId="0" sqref="M77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.3"/>
@@ -1828,7 +1868,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="54.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="26"/>
@@ -1914,7 +1954,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -1944,67 +1984,67 @@
     </row>
     <row r="10" s="12" customFormat="true" ht="73.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2012,72 +2052,72 @@
         <v>31</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>37</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N11" s="13" t="s">
         <v>40</v>
       </c>
       <c r="O11" s="13" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q11" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="S11" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="U11" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="V11" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="U12" s="22"/>
     </row>
@@ -2087,7 +2127,7 @@
         <v>epsh:P13</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>43</v>
@@ -2096,10 +2136,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I13" s="1" t="str">
         <f aca="false">LEFT(H13,1)</f>
@@ -2110,7 +2150,7 @@
         <v/>
       </c>
       <c r="K13" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2119,7 +2159,7 @@
         <v>epsh:P14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>43</v>
@@ -2129,7 +2169,7 @@
       </c>
       <c r="E14" s="1"/>
       <c r="G14" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="1" t="str">
@@ -2141,7 +2181,7 @@
         <v/>
       </c>
       <c r="K14" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N14" s="5"/>
       <c r="S14" s="1"/>
@@ -2152,7 +2192,7 @@
         <v>epsh:P15</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>43</v>
@@ -2161,10 +2201,10 @@
         <v>4</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I15" s="1" t="str">
         <f aca="false">LEFT(H15,1)</f>
@@ -2175,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N15" s="5"/>
     </row>
@@ -2185,7 +2225,7 @@
         <v>epsh:P16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>43</v>
@@ -2194,10 +2234,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I16" s="1" t="str">
         <f aca="false">LEFT(H16,1)</f>
@@ -2208,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N16" s="23"/>
     </row>
@@ -2218,7 +2258,7 @@
         <v>epsh:P17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>43</v>
@@ -2227,10 +2267,10 @@
         <v>6</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I17" s="1" t="str">
         <f aca="false">LEFT(H17,1)</f>
@@ -2241,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N17" s="23"/>
     </row>
@@ -2251,7 +2291,7 @@
         <v>epsh:P18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>43</v>
@@ -2260,10 +2300,10 @@
         <v>7</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I18" s="1" t="str">
         <f aca="false">LEFT(H18,1)</f>
@@ -2274,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N18" s="23"/>
     </row>
@@ -2284,7 +2324,7 @@
         <v>epsh:P19</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>43</v>
@@ -2297,7 +2337,7 @@
         <v>47</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I19" s="1" t="str">
         <f aca="false">LEFT(H19,1)</f>
@@ -2319,7 +2359,7 @@
         <v>epsh:P20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>43</v>
@@ -2332,7 +2372,7 @@
         <v>47</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I20" s="1" t="str">
         <f aca="false">LEFT(H20,1)</f>
@@ -2354,7 +2394,7 @@
         <v>epsh:P21</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>43</v>
@@ -2367,7 +2407,7 @@
         <v>47</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I21" s="1" t="str">
         <f aca="false">LEFT(H21,1)</f>
@@ -2389,7 +2429,7 @@
         <v>epsh:P22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>43</v>
@@ -2402,7 +2442,7 @@
         <v>47</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I22" s="1" t="str">
         <f aca="false">LEFT(H22,1)</f>
@@ -2424,7 +2464,7 @@
         <v>epsh:P23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>43</v>
@@ -2437,7 +2477,7 @@
         <v>47</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I23" s="1" t="str">
         <f aca="false">LEFT(H23,1)</f>
@@ -2447,7 +2487,7 @@
         <f aca="false">IF(OR(RIGHT(H23,1) = "n", RIGHT(H23,1) = "*"),"",RIGHT(H23,1))</f>
         <v>1</v>
       </c>
-      <c r="M23" s="25" t="s">
+      <c r="M23" s="5" t="s">
         <v>86</v>
       </c>
       <c r="N23" s="23"/>
@@ -2459,7 +2499,7 @@
         <v>epsh:P24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>43</v>
@@ -2472,7 +2512,7 @@
         <v>47</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I24" s="1" t="str">
         <f aca="false">LEFT(H24,1)</f>
@@ -2494,7 +2534,7 @@
         <v>epsh:P25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>43</v>
@@ -2507,7 +2547,7 @@
         <v>47</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I25" s="1" t="str">
         <f aca="false">LEFT(H25,1)</f>
@@ -2529,7 +2569,7 @@
         <v>epsh:P26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>43</v>
@@ -2543,7 +2583,7 @@
         <v>47</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I26" s="1" t="str">
         <f aca="false">LEFT(H26,1)</f>
@@ -2572,7 +2612,7 @@
         <v>epsh:P27</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>43</v>
@@ -2584,7 +2624,7 @@
         <v>47</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I27" s="1" t="str">
         <f aca="false">LEFT(H27,1)</f>
@@ -2604,7 +2644,7 @@
         <v>epsh:P28</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>43</v>
@@ -2616,7 +2656,7 @@
         <v>47</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I28" s="1" t="str">
         <f aca="false">LEFT(H28,1)</f>
@@ -2636,7 +2676,7 @@
         <v>epsh:P29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>43</v>
@@ -2645,10 +2685,10 @@
         <v>18</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I29" s="1" t="str">
         <f aca="false">LEFT(H29,1)</f>
@@ -2665,7 +2705,7 @@
         <v>epsh:P30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>43</v>
@@ -2678,7 +2718,7 @@
         <v>47</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I30" s="1" t="str">
         <f aca="false">LEFT(H30,1)</f>
@@ -2699,7 +2739,7 @@
         <v>epsh:P31</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>43</v>
@@ -2712,7 +2752,7 @@
         <v>47</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I31" s="1" t="str">
         <f aca="false">LEFT(H31,1)</f>
@@ -2725,7 +2765,7 @@
     </row>
     <row r="34" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="U34" s="22"/>
     </row>
@@ -2735,7 +2775,7 @@
         <v>epsh:P35</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>51</v>
@@ -2744,10 +2784,10 @@
         <v>1</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I35" s="1" t="str">
         <f aca="false">LEFT(H35,1)</f>
@@ -2758,7 +2798,7 @@
         <v/>
       </c>
       <c r="K35" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2767,7 +2807,7 @@
         <v>epsh:P36</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>51</v>
@@ -2777,10 +2817,10 @@
       </c>
       <c r="E36" s="1"/>
       <c r="G36" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I36" s="1" t="str">
         <f aca="false">LEFT(H36,1)</f>
@@ -2791,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="S36" s="1"/>
     </row>
@@ -2801,7 +2841,7 @@
         <v>epsh:P37</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>51</v>
@@ -2810,10 +2850,10 @@
         <v>3</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I37" s="1" t="str">
         <f aca="false">LEFT(H37,1)</f>
@@ -2824,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,7 +2873,7 @@
         <v>epsh:P38</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>51</v>
@@ -2842,10 +2882,10 @@
         <v>4</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I38" s="1" t="str">
         <f aca="false">LEFT(H38,1)</f>
@@ -2856,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,7 +2905,7 @@
         <v>epsh:P39</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>51</v>
@@ -2877,7 +2917,7 @@
         <v>47</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I39" s="1" t="str">
         <f aca="false">LEFT(H39,1)</f>
@@ -2897,7 +2937,7 @@
         <v>epsh:P40</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>51</v>
@@ -2909,7 +2949,7 @@
         <v>47</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I40" s="1" t="str">
         <f aca="false">LEFT(H40,1)</f>
@@ -2929,7 +2969,7 @@
         <v>epsh:P41</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>51</v>
@@ -2941,7 +2981,7 @@
         <v>47</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I41" s="1" t="str">
         <f aca="false">LEFT(H41,1)</f>
@@ -2961,7 +3001,7 @@
         <v>epsh:P42</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>51</v>
@@ -2973,7 +3013,7 @@
         <v>47</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I42" s="1" t="str">
         <f aca="false">LEFT(H42,1)</f>
@@ -2993,7 +3033,7 @@
         <v>epsh:P43</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>51</v>
@@ -3005,7 +3045,7 @@
         <v>47</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I43" s="1" t="str">
         <f aca="false">LEFT(H43,1)</f>
@@ -3025,7 +3065,7 @@
         <v>epsh:P44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>51</v>
@@ -3037,7 +3077,7 @@
         <v>47</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I44" s="1" t="str">
         <f aca="false">LEFT(H44,1)</f>
@@ -3057,7 +3097,7 @@
         <v>epsh:P45</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>51</v>
@@ -3087,7 +3127,7 @@
         <v>epsh:P46</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>51</v>
@@ -3096,10 +3136,10 @@
         <v>12</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I46" s="1" t="str">
         <f aca="false">LEFT(H46,1)</f>
@@ -3110,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3119,7 +3159,7 @@
         <v>epsh:P47</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>51</v>
@@ -3149,7 +3189,7 @@
         <v>epsh:P48</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>51</v>
@@ -3161,7 +3201,7 @@
         <v>47</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I48" s="1" t="str">
         <f aca="false">LEFT(H48,1)</f>
@@ -3181,7 +3221,7 @@
         <v>epsh:P49</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>51</v>
@@ -3193,7 +3233,7 @@
         <v>47</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I49" s="1" t="str">
         <f aca="false">LEFT(H49,1)</f>
@@ -3213,7 +3253,7 @@
         <v>epsh:P50</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>51</v>
@@ -3225,7 +3265,7 @@
         <v>47</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I50" s="1" t="str">
         <f aca="false">LEFT(H50,1)</f>
@@ -3245,7 +3285,7 @@
         <v>epsh:P51</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>51</v>
@@ -3257,7 +3297,7 @@
         <v>47</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I51" s="1" t="str">
         <f aca="false">LEFT(H51,1)</f>
@@ -3277,7 +3317,7 @@
         <v>epsh:P52</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>51</v>
@@ -3289,7 +3329,7 @@
         <v>47</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I52" s="1" t="str">
         <f aca="false">LEFT(H52,1)</f>
@@ -3309,7 +3349,7 @@
         <v>epsh:P53</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>51</v>
@@ -3321,7 +3361,7 @@
         <v>47</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I53" s="1" t="str">
         <f aca="false">LEFT(H53,1)</f>
@@ -3341,7 +3381,7 @@
         <v>epsh:P54</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>51</v>
@@ -3353,7 +3393,7 @@
         <v>47</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I54" s="1" t="str">
         <f aca="false">LEFT(H54,1)</f>
@@ -3373,7 +3413,7 @@
         <v>epsh:P55</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>51</v>
@@ -3385,7 +3425,7 @@
         <v>47</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I55" s="1" t="str">
         <f aca="false">LEFT(H55,1)</f>
@@ -3405,7 +3445,7 @@
         <v>epsh:P56</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>51</v>
@@ -3417,7 +3457,7 @@
         <v>47</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I56" s="1" t="str">
         <f aca="false">LEFT(H56,1)</f>
@@ -3437,7 +3477,7 @@
         <v>epsh:P57</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>51</v>
@@ -3449,7 +3489,7 @@
         <v>47</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I57" s="1" t="str">
         <f aca="false">LEFT(H57,1)</f>
@@ -3469,7 +3509,7 @@
         <v>epsh:P58</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>51</v>
@@ -3481,7 +3521,7 @@
         <v>47</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I58" s="1" t="str">
         <f aca="false">LEFT(H58,1)</f>
@@ -3501,7 +3541,7 @@
         <v>epsh:P59</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>51</v>
@@ -3513,7 +3553,7 @@
         <v>47</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I59" s="1" t="str">
         <f aca="false">LEFT(H59,1)</f>
@@ -3533,7 +3573,7 @@
         <v>epsh:P60</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>51</v>
@@ -3542,10 +3582,10 @@
         <v>26</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I60" s="1" t="str">
         <f aca="false">LEFT(H60,1)</f>
@@ -3556,7 +3596,7 @@
         <v>1</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3565,7 +3605,7 @@
         <v>epsh:P61</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>51</v>
@@ -3577,7 +3617,7 @@
         <v>47</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I61" s="1" t="str">
         <f aca="false">LEFT(H61,1)</f>
@@ -3593,7 +3633,7 @@
     </row>
     <row r="63" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="21" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="U63" s="22"/>
     </row>
@@ -3603,9 +3643,9 @@
         <v>epsh:P64</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C64" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D64" s="1" t="n">
@@ -3615,10 +3655,14 @@
         <v>47</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I64" s="1" t="str">
         <f aca="false">LEFT(H64,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J64" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H64,1) = "n", RIGHT(H64,1) = "*"),"",RIGHT(H64,1))</f>
         <v>1</v>
       </c>
       <c r="M64" s="5" t="s">
@@ -3631,9 +3675,9 @@
         <v>epsh:P65</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="C65" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D65" s="1" t="n">
@@ -3643,10 +3687,14 @@
         <v>47</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I65" s="1" t="str">
         <f aca="false">LEFT(H65,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J65" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H65,1) = "n", RIGHT(H65,1) = "*"),"",RIGHT(H65,1))</f>
         <v>1</v>
       </c>
       <c r="M65" s="5" t="s">
@@ -3659,7 +3707,7 @@
         <v>epsh:P66</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>62</v>
@@ -3671,29 +3719,33 @@
         <v>47</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I66" s="1" t="str">
         <f aca="false">LEFT(H66,1)</f>
         <v>0</v>
       </c>
+      <c r="J66" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H66,1) = "n", RIGHT(H66,1) = "*"),"",RIGHT(H66,1))</f>
+        <v>1</v>
+      </c>
       <c r="M66" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="68" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="U68" s="22"/>
     </row>
-    <row r="69" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A69))</f>
         <v>epsh:P69</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>55</v>
@@ -3702,19 +3754,27 @@
         <v>1</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="I69" s="1" t="str">
+        <f aca="false">LEFT(H69,1)</f>
+        <v/>
+      </c>
+      <c r="J69" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H69,1) = "n", RIGHT(H69,1) = "*"),"",RIGHT(H69,1))</f>
+        <v/>
       </c>
       <c r="K69" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A70))</f>
         <v>epsh:P70</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>55</v>
@@ -3725,17 +3785,25 @@
       <c r="G70" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="I70" s="1" t="str">
+        <f aca="false">LEFT(H70,1)</f>
+        <v/>
+      </c>
+      <c r="J70" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H70,1) = "n", RIGHT(H70,1) = "*"),"",RIGHT(H70,1))</f>
+        <v/>
+      </c>
       <c r="M70" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A71))</f>
         <v>epsh:P71</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>55</v>
@@ -3746,17 +3814,25 @@
       <c r="G71" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="I71" s="1" t="str">
+        <f aca="false">LEFT(H71,1)</f>
+        <v/>
+      </c>
+      <c r="J71" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H71,1) = "n", RIGHT(H71,1) = "*"),"",RIGHT(H71,1))</f>
+        <v/>
+      </c>
       <c r="M71" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A72))</f>
         <v>epsh:P72</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>55</v>
@@ -3765,19 +3841,27 @@
         <v>4</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="I72" s="1" t="str">
+        <f aca="false">LEFT(H72,1)</f>
+        <v/>
+      </c>
+      <c r="J72" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H72,1) = "n", RIGHT(H72,1) = "*"),"",RIGHT(H72,1))</f>
+        <v/>
       </c>
       <c r="K72" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A73))</f>
         <v>epsh:P73</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>55</v>
@@ -3786,19 +3870,27 @@
         <v>5</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="I73" s="1" t="str">
+        <f aca="false">LEFT(H73,1)</f>
+        <v/>
+      </c>
+      <c r="J73" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H73,1) = "n", RIGHT(H73,1) = "*"),"",RIGHT(H73,1))</f>
+        <v/>
       </c>
       <c r="K73" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A74))</f>
         <v>epsh:P74</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>55</v>
@@ -3807,10 +3899,88 @@
         <v>6</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
+      </c>
+      <c r="I74" s="1" t="str">
+        <f aca="false">LEFT(H74,1)</f>
+        <v/>
+      </c>
+      <c r="J74" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H74,1) = "n", RIGHT(H74,1) = "*"),"",RIGHT(H74,1))</f>
+        <v/>
       </c>
       <c r="K74" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" s="21" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="U76" s="22"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A77))</f>
+        <v>epsh:P77</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I77" s="1" t="str">
+        <f aca="false">LEFT(H77,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J77" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H77,1) = "n", RIGHT(H77,1) = "*"),"",RIGHT(H77,1))</f>
+        <v>1</v>
+      </c>
+      <c r="M77" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="str">
+        <f aca="false">CONCATENATE("epsh:P",ROW(A78))</f>
+        <v>epsh:P78</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I78" s="1" t="str">
+        <f aca="false">LEFT(H78,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J78" s="0" t="str">
+        <f aca="false">IF(OR(RIGHT(H78,1) = "n", RIGHT(H78,1) = "*"),"",RIGHT(H78,1))</f>
+        <v>1</v>
+      </c>
+      <c r="M78" s="25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>